<commit_message>
header to excel file has been added.
</commit_message>
<xml_diff>
--- a/GeoLocation/obj/Release/net6.0/PubTmp/Out/wwwroot/Upload/schoolsDataLess.xlsx
+++ b/GeoLocation/obj/Release/net6.0/PubTmp/Out/wwwroot/Upload/schoolsDataLess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_rajabian\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF22F64E-22C9-4707-892B-2110900CBB66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938B7B3D-37D9-42D7-BBB2-E250281A4EBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{A713C247-CCCB-4DDE-BADF-3C6323A70C4C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="232">
   <si>
     <t>استان</t>
   </si>
@@ -595,6 +595,132 @@
   </si>
   <si>
     <t>سفيران دانش</t>
+  </si>
+  <si>
+    <t>البرز</t>
+  </si>
+  <si>
+    <t>کرج ناحيه 4</t>
+  </si>
+  <si>
+    <t>شهيدان  هداوند</t>
+  </si>
+  <si>
+    <t>حصار ک بالا خيابان آقارضايي آموزشگاه شهيدان هداوند2</t>
+  </si>
+  <si>
+    <t>شهداي کمالشهر</t>
+  </si>
+  <si>
+    <t>کمالشهر_خ وليعصرجنوبي _خ شهدا</t>
+  </si>
+  <si>
+    <t>شهيد صياد شيرازي</t>
+  </si>
+  <si>
+    <t>کمالشهر جنب مسجد علي ابن ابي طالب- مدرسه ش صياد شيرازي</t>
+  </si>
+  <si>
+    <t>شهيدستارلطفي</t>
+  </si>
+  <si>
+    <t>کيانمهر</t>
+  </si>
+  <si>
+    <t>هنرستان امام خميني (ره )(1)</t>
+  </si>
+  <si>
+    <t>فاز4مهرشهر_بلوار گلها _چهارراه هنرستان خ 406شرقي-پ192</t>
+  </si>
+  <si>
+    <t>حضرت مريم (1)</t>
+  </si>
+  <si>
+    <t>مهرشهر_بلوارارم _بلواردانش _خ 100_خ مريم</t>
+  </si>
+  <si>
+    <t>شهيد شهسواري(2)</t>
+  </si>
+  <si>
+    <t>کرج- حصارک پايين -رضاشهر-انتهاي خيابان فروردين</t>
+  </si>
+  <si>
+    <t>لقمان حکيم(1)</t>
+  </si>
+  <si>
+    <t>کرج-پيشاهنگي-گلدشت</t>
+  </si>
+  <si>
+    <t>هدايت</t>
+  </si>
+  <si>
+    <t>شهيد پرورش</t>
+  </si>
+  <si>
+    <t>شهرک کيان مهر-خ نبرد اهواز - مدرسه شهيدمحمدپرورشي</t>
+  </si>
+  <si>
+    <t>امام رضا(ع )2</t>
+  </si>
+  <si>
+    <t>جاده قزلحصارروبروي بي سيم شهرک سهرابيه</t>
+  </si>
+  <si>
+    <t>شهيد باهنر</t>
+  </si>
+  <si>
+    <t>کيان مهر ميدان مهرگان بوستان هفتم</t>
+  </si>
+  <si>
+    <t>وحدت اسلامي (1)</t>
+  </si>
+  <si>
+    <t>حصارک بالا_روبروي مجتمع ورزشي ايثار</t>
+  </si>
+  <si>
+    <t>وليعصر(عج)</t>
+  </si>
+  <si>
+    <t>کيانمهر_بلواراميرکبير_جنب ميدان امام خميني (ره )</t>
+  </si>
+  <si>
+    <t>صداقت</t>
+  </si>
+  <si>
+    <t>کرج-خرمدشت-ميثم يک-بهار اول-پلاک37</t>
+  </si>
+  <si>
+    <t>فرازين</t>
+  </si>
+  <si>
+    <t>کرج-فاز2مهرشهر-بلوار شهرداري-خيابان202-پلاک382/1 پيش و ابتدايي فرازين</t>
+  </si>
+  <si>
+    <t>حضرت امير(ع)</t>
+  </si>
+  <si>
+    <t>کرج-خيابان درختي-نرسيده به سه راه تهران-پلاک325-متوسطه دوره اول حضرت امير(ع)</t>
+  </si>
+  <si>
+    <t>شادان</t>
+  </si>
+  <si>
+    <t>کرج-حصارک - خيابان برزنت-90دستگاه اول-پلاک34-متوسطه اول شادان</t>
+  </si>
+  <si>
+    <t>عصر تلاش</t>
+  </si>
+  <si>
+    <t>نيوشا</t>
+  </si>
+  <si>
+    <t>کرج-خيايان45متري گلشهر-کوچه مينا-پلاک35-متوسطه اول نيوشا</t>
+  </si>
+  <si>
+    <t>انديشه</t>
+  </si>
+  <si>
+    <t>کرج-45متري گلشهر-آذرشرقي-پلاک14-کاردانش انديشه</t>
   </si>
 </sst>
 </file>
@@ -981,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8AC05DB-C500-4B8D-9656-1DE3CF56854A}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:XFD96"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,8 +1191,8 @@
       <c r="I2" s="2">
         <v>33710445</v>
       </c>
-      <c r="J2" s="2">
-        <v>561755413</v>
+      <c r="J2">
+        <v>5616677351</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>19</v>
@@ -1100,8 +1226,8 @@
       <c r="I3" s="2">
         <v>33711077</v>
       </c>
-      <c r="J3" s="2">
-        <v>561573589</v>
+      <c r="J3">
+        <v>5614858433</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>24</v>
@@ -1135,8 +1261,8 @@
       <c r="I4" s="2">
         <v>3351040</v>
       </c>
-      <c r="J4" s="2">
-        <v>56149</v>
+      <c r="J4">
+        <v>5615869888</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>28</v>
@@ -1170,8 +1296,8 @@
       <c r="I5" s="2">
         <v>33253330</v>
       </c>
-      <c r="J5" s="2">
-        <v>561475493</v>
+      <c r="J5">
+        <v>5614714457</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>32</v>
@@ -1205,8 +1331,8 @@
       <c r="I6" s="2">
         <v>2238667</v>
       </c>
-      <c r="J6" s="2">
-        <v>561366376</v>
+      <c r="J6">
+        <v>5619647774</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>34</v>
@@ -1240,8 +1366,8 @@
       <c r="I7" s="2">
         <v>4441311</v>
       </c>
-      <c r="J7" s="2">
-        <v>561593683</v>
+      <c r="J7">
+        <v>5614786795</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>36</v>
@@ -1275,8 +1401,8 @@
       <c r="I8" s="2">
         <v>33628400</v>
       </c>
-      <c r="J8" s="2">
-        <v>561985656</v>
+      <c r="J8">
+        <v>5619744199</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>39</v>
@@ -1310,8 +1436,8 @@
       <c r="I9" s="2">
         <v>33629940</v>
       </c>
-      <c r="J9" s="2">
-        <v>561976349</v>
+      <c r="J9">
+        <v>5618645137</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>42</v>
@@ -1345,8 +1471,8 @@
       <c r="I10" s="2">
         <v>4442573</v>
       </c>
-      <c r="J10" s="2">
-        <v>561566</v>
+      <c r="J10">
+        <v>5616914758</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>44</v>
@@ -1380,8 +1506,8 @@
       <c r="I11" s="2">
         <v>2247452</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>32</v>
+      <c r="J11">
+        <v>5616667133</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>48</v>
@@ -1415,8 +1541,8 @@
       <c r="I12" s="2">
         <v>2242610</v>
       </c>
-      <c r="J12" s="2">
-        <v>561473</v>
+      <c r="J12">
+        <v>5615945674</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>50</v>
@@ -1450,8 +1576,8 @@
       <c r="I13" s="2">
         <v>33713906</v>
       </c>
-      <c r="J13" s="2">
-        <v>561578851</v>
+      <c r="J13">
+        <v>5615853684</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>53</v>
@@ -1485,8 +1611,8 @@
       <c r="I14" s="2">
         <v>2240149</v>
       </c>
-      <c r="J14" s="2">
-        <v>561477</v>
+      <c r="J14">
+        <v>5615938591</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>55</v>
@@ -1520,8 +1646,8 @@
       <c r="I15" s="2">
         <v>7712235</v>
       </c>
-      <c r="J15" s="2">
-        <v>561576</v>
+      <c r="J15">
+        <v>5616677373</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>57</v>
@@ -1555,8 +1681,8 @@
       <c r="I16" s="2">
         <v>6624534</v>
       </c>
-      <c r="J16" s="2">
-        <v>561976</v>
+      <c r="J16">
+        <v>5619831869</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>59</v>
@@ -1590,8 +1716,8 @@
       <c r="I17" s="2">
         <v>33440410</v>
       </c>
-      <c r="J17" s="2">
-        <v>561683113</v>
+      <c r="J17">
+        <v>5618956315</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>61</v>
@@ -1625,8 +1751,8 @@
       <c r="I18" s="2">
         <v>4449300</v>
       </c>
-      <c r="J18" s="2">
-        <v>561665399</v>
+      <c r="J18">
+        <v>5616914654</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>44</v>
@@ -1660,8 +1786,8 @@
       <c r="I19" s="2">
         <v>33712383</v>
       </c>
-      <c r="J19" s="2">
-        <v>561479464</v>
+      <c r="J19">
+        <v>5618954116</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>64</v>
@@ -1695,8 +1821,8 @@
       <c r="I20" s="2">
         <v>33746562</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>32</v>
+      <c r="J20">
+        <v>5618956315</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>66</v>
@@ -1730,8 +1856,8 @@
       <c r="I21" s="2">
         <v>33442873</v>
       </c>
-      <c r="J21" s="2">
-        <v>561566533</v>
+      <c r="J21">
+        <v>5613917133</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>68</v>
@@ -1765,8 +1891,8 @@
       <c r="I22" s="2">
         <v>2237481</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>32</v>
+      <c r="J22">
+        <v>5616695198</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>70</v>
@@ -1800,8 +1926,8 @@
       <c r="I23" s="2">
         <v>33633767</v>
       </c>
-      <c r="J23" s="2">
-        <v>561984819</v>
+      <c r="J23">
+        <v>5615955997</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>72</v>
@@ -1835,8 +1961,8 @@
       <c r="I24" s="2">
         <v>33442874</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>32</v>
+      <c r="J24">
+        <v>5614854416</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>74</v>
@@ -1870,8 +1996,8 @@
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>32</v>
+      <c r="J25">
+        <v>5613643175</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>32</v>
@@ -1905,8 +2031,8 @@
       <c r="I26" s="2">
         <v>4440800</v>
       </c>
-      <c r="J26" s="2">
-        <v>561479369</v>
+      <c r="J26">
+        <v>5614788353</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>77</v>
@@ -1940,8 +2066,8 @@
       <c r="I27" s="2">
         <v>33444561</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>32</v>
+      <c r="J27">
+        <v>5616921415</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>79</v>
@@ -1975,8 +2101,8 @@
       <c r="I28" s="2">
         <v>33</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>32</v>
+      <c r="J28">
+        <v>5615749433</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -2010,8 +2136,8 @@
       <c r="I29" s="2">
         <v>33</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>32</v>
+      <c r="J29">
+        <v>5619843437</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>83</v>
@@ -2045,8 +2171,8 @@
       <c r="I30" s="2">
         <v>33234815</v>
       </c>
-      <c r="J30" s="2">
-        <v>561974538</v>
+      <c r="J30">
+        <v>5619813471</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>85</v>
@@ -2080,8 +2206,8 @@
       <c r="I31" s="2">
         <v>7714777</v>
       </c>
-      <c r="J31" s="2">
-        <v>561576344</v>
+      <c r="J31">
+        <v>5614975479</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>87</v>
@@ -2115,8 +2241,8 @@
       <c r="I32" s="2">
         <v>33710450</v>
       </c>
-      <c r="J32" s="2">
-        <v>561575163</v>
+      <c r="J32">
+        <v>5617755983</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>89</v>
@@ -2150,8 +2276,8 @@
       <c r="I33" s="2">
         <v>4462457</v>
       </c>
-      <c r="J33" s="2">
-        <v>561593719</v>
+      <c r="J33">
+        <v>5616744552</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>91</v>
@@ -2185,8 +2311,8 @@
       <c r="I34" s="2">
         <v>4445260</v>
       </c>
-      <c r="J34" s="2">
-        <v>561487</v>
+      <c r="J34">
+        <v>5617671652</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>93</v>
@@ -4360,6 +4486,741 @@
       </c>
       <c r="K96" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I97" s="2">
+        <v>4552018</v>
+      </c>
+      <c r="J97" s="2">
+        <v>319777333</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I98" s="2">
+        <v>4703847</v>
+      </c>
+      <c r="J98" s="2">
+        <v>319976577</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I99" s="2">
+        <v>34703847</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I101" s="2">
+        <v>3528485</v>
+      </c>
+      <c r="J101" s="2">
+        <v>318383464</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I102" s="2">
+        <v>3408607</v>
+      </c>
+      <c r="J102" s="2">
+        <v>318579855</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I103" s="2">
+        <v>34662060</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K103" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I104" s="2">
+        <v>34801188</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I106" s="2">
+        <v>33214848</v>
+      </c>
+      <c r="J106" s="2">
+        <v>123454</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I107" s="2">
+        <v>3315356</v>
+      </c>
+      <c r="J107" s="2">
+        <v>318695759</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I108" s="2">
+        <v>33203180</v>
+      </c>
+      <c r="J108" s="2">
+        <v>318761748</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I109" s="2">
+        <v>4553805</v>
+      </c>
+      <c r="J109" s="2">
+        <v>319767745</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I110" s="2">
+        <v>3212728</v>
+      </c>
+      <c r="J110" s="2">
+        <v>318761748</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I111" s="2">
+        <v>34801130</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I112" s="2">
+        <v>33420115</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I113" s="2">
+        <v>3509123</v>
+      </c>
+      <c r="J113" s="2">
+        <v>313965359</v>
+      </c>
+      <c r="K113" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I114" s="2">
+        <v>34613059</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I115" s="2">
+        <v>34516780</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I116" s="2">
+        <v>33513094</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I117" s="2">
+        <v>4641296</v>
+      </c>
+      <c r="J117" s="2">
+        <v>313891491</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>